<commit_message>
commit on 'Yiyuan Zhang'
</commit_message>
<xml_diff>
--- a/cuda_convolution/cuda_data.xlsx
+++ b/cuda_convolution/cuda_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\WeChat Files\zyy2001717\FileStorage\File\2021-09\cuda_convolution\Parallel-convolution\cuda_convolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEC58DE-1A11-401F-981A-967AABC63DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2876C6C6-FFFD-4B82-91EF-B522258DDE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="360" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.000_);[Red]\(0.000\)"/>
+    <numFmt numFmtId="176" formatCode="0.000_);[Red]\(0.000\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -190,7 +190,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -243,9 +243,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>串并行计算加速比与计算规模变化图</a:t>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>kernel=3,5,9,12,15, img=512</a:t>
             </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -280,17 +281,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12798648864544107"/>
-          <c:y val="4.527036995629586E-2"/>
-          <c:w val="0.83491206207919666"/>
-          <c:h val="0.7243315348318633"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -311,10 +302,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$Y$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>0.000_);[Red]\(0.000\)</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>16.099</c:v>
                 </c:pt>
@@ -330,70 +321,13 @@
                 <c:pt idx="4">
                   <c:v>318.36500000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>61.154000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>152.56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>489.24200000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>866.04899999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1600.65</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>268.35700000000003</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>626.28499999999997</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1952.97</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>3443.63</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>5396.59</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>988.16499999999996</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="General">
-                  <c:v>8241</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>14514.5</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="General">
-                  <c:v>22420.2</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>4134.59</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="General">
-                  <c:v>10717</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="General">
-                  <c:v>32826.9</c:v>
-                </c:pt>
-                <c:pt idx="22" formatCode="General">
-                  <c:v>58481.7</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="General">
-                  <c:v>90899.6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-589E-4908-B460-F688DC1A2F28}"/>
+              <c16:uniqueId val="{00000000-C19D-404A-B50D-B5482743C676}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -414,10 +348,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$Y$3</c:f>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>0.000_);[Red]\(0.000\)</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.219</c:v>
                 </c:pt>
@@ -433,70 +367,13 @@
                 <c:pt idx="4">
                   <c:v>7.7119999999999997</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.621</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.8010000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.577999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>21.052</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.442</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>2.6789999999999998</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>6.67</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21.855</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>36.21</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>56.497</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>10.254</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="General">
-                  <c:v>87.84</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>203.989</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="General">
-                  <c:v>450.52699999999999</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>91.947000000000003</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="General">
-                  <c:v>239.792</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="General">
-                  <c:v>348.65100000000001</c:v>
-                </c:pt>
-                <c:pt idx="22" formatCode="General">
-                  <c:v>764.43700000000001</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="General">
-                  <c:v>1291.0999999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-589E-4908-B460-F688DC1A2F28}"/>
+              <c16:uniqueId val="{00000001-C19D-404A-B50D-B5482743C676}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -509,11 +386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1085824767"/>
-        <c:axId val="1085827263"/>
+        <c:axId val="883203823"/>
+        <c:axId val="883207983"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1085824767"/>
+        <c:axId val="883203823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,7 +432,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1085827263"/>
+        <c:crossAx val="883207983"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -563,7 +440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1085827263"/>
+        <c:axId val="883207983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,7 +491,1499 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1085824767"/>
+        <c:crossAx val="883203823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>kernel=3,5,9,12,15</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>, img=1024</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000_);[Red]\(0.000\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61.154000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>489.24200000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>866.04899999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD74-4250-B80E-BCE9AC12D4E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.000_);[Red]\(0.000\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.621</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.577999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AD74-4250-B80E-BCE9AC12D4E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="890776639"/>
+        <c:axId val="890777471"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="890776639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="890777471"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="890777471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000_);[Red]\(0.000\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="890776639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>kernel=3,5,9,12,15, img=2048</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000_);[Red]\(0.000\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>268.35700000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>626.28499999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1952.97</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>3443.63</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>5396.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F754-40A9-B04A-656EEF51D5A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.6789999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.67</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000_);[Red]\(0.000\)">
+                  <c:v>21.855</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F754-40A9-B04A-656EEF51D5A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="894448815"/>
+        <c:axId val="894450479"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="894448815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="894450479"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="894450479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="894448815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>kernel=3,5,9,12,15, img=4096</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$T$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>988.16499999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14514.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22420.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5334-46DD-BB95-231F0EE4E472}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.254</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>203.989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>450.52699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5334-46DD-BB95-231F0EE4E472}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="947139839"/>
+        <c:axId val="947140255"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="947139839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="947140255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="947140255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="947139839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>kernel=3,5,9,12,15, img=8192</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$Y$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4134.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32826.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58481.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90899.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BD0-4CE5-B817-DB6C8725B233}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$3:$Y$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>91.947000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>239.792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>348.65100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>764.43700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1291.0999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7BD0-4CE5-B817-DB6C8725B233}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="950623711"/>
+        <c:axId val="950615807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="950623711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="950615807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="950615807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="950623711"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -741,7 +2110,2231 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1262,22 +4855,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>465257</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>2199</xdr:rowOff>
+      <xdr:colOff>311393</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>148735</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>380997</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>73270</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>18316</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144339</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3">
+        <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DB10F4A-23BF-4058-91C1-44A4062DB097}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{672D55AC-A435-476A-8FB7-2C660A2F7BEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,6 +4883,150 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>322385</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>29308</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>100378</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7E1479-55FC-466A-BF69-C0F5EE6C798F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>512885</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>183174</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>158994</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F837492D-B020-4E73-B190-3B47776F99F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>622788</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>170717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>293077</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>166321</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="图表 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9139363D-EE22-4A19-A452-B4DCE2982A6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>549520</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>178043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>300404</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>173647</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="图表 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0026EB45-F243-4599-9B6A-2F5B059F7728}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1564,7 +5301,7 @@
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="R36" activeCellId="1" sqref="T37 R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>